<commit_message>
Fix 9956 removal date; TICC-292
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Participant identifier schemes v8.7.xlsx
+++ b/work-in-progress/Peppol Code Lists - Participant identifier schemes v8.7.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\peppol-edec-codelists\work-in-progress\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A5B6E5-0624-4AD9-8EF0-18B0F5675468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE7D8C8-2B79-4BC0-8EE6-8F25720BF94B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="780" windowWidth="15180" windowHeight="20010" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4245" yWindow="4245" windowWidth="21600" windowHeight="12645" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Participant Identifier Scheme" sheetId="1" r:id="rId1"/>
@@ -2752,7 +2752,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D94" sqref="D94"/>
+      <selection pane="bottomRight" activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14885,7 +14885,7 @@
         <v>459</v>
       </c>
       <c r="I93" s="22">
-        <v>45230</v>
+        <v>45292</v>
       </c>
       <c r="J93" s="19" t="s">
         <v>330</v>

</xml_diff>

<commit_message>
9956 removal date 31.12.23 instead of 1.1.24; TICC-292
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Participant identifier schemes v8.7.xlsx
+++ b/work-in-progress/Peppol Code Lists - Participant identifier schemes v8.7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE7D8C8-2B79-4BC0-8EE6-8F25720BF94B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9829C12-54A8-410E-8EA3-6987A8A78951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4245" yWindow="4245" windowWidth="21600" windowHeight="12645" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Participant Identifier Scheme" sheetId="1" r:id="rId1"/>
@@ -2752,7 +2752,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A93" sqref="A93"/>
+      <selection pane="bottomRight" activeCell="I94" sqref="I94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14885,7 +14885,7 @@
         <v>459</v>
       </c>
       <c r="I93" s="22">
-        <v>45292</v>
+        <v>45291</v>
       </c>
       <c r="J93" s="19" t="s">
         <v>330</v>

</xml_diff>